<commit_message>
adding more features to our assmbler
</commit_message>
<xml_diff>
--- a/additional_information/ALU_7bits.xlsx
+++ b/additional_information/ALU_7bits.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>EN_OUT</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>A|DB</t>
+  </si>
+  <si>
+    <t>A++</t>
+  </si>
+  <si>
+    <t>A--</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +791,58 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding stack pointer and more intersting commands like jsr ret pha pla etc..
</commit_message>
<xml_diff>
--- a/additional_information/ALU_7bits.xlsx
+++ b/additional_information/ALU_7bits.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>EN_OUT</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>A--</t>
+  </si>
+  <si>
+    <t>db--</t>
+  </si>
+  <si>
+    <t>db++</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,6 +849,58 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>